<commit_message>
seems to read in teachers
</commit_message>
<xml_diff>
--- a/sampleClassToArrange.xlsx
+++ b/sampleClassToArrange.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arutf\Documents\classOrganization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9F85385-418B-4D14-AAB1-4C175FD13676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A732A07B-3CD9-4316-AAE7-CC784F88AF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Teachers</t>
   </si>
@@ -64,6 +64,51 @@
   </si>
   <si>
     <t>Special circumstances</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>Three</t>
+  </si>
+  <si>
+    <t>Four</t>
+  </si>
+  <si>
+    <t>Five</t>
+  </si>
+  <si>
+    <t>Six</t>
+  </si>
+  <si>
+    <t>Seven</t>
+  </si>
+  <si>
+    <t>Eight</t>
+  </si>
+  <si>
+    <t>Nine</t>
+  </si>
+  <si>
+    <t>Ten</t>
+  </si>
+  <si>
+    <t>Eleven</t>
+  </si>
+  <si>
+    <t>Twelve</t>
+  </si>
+  <si>
+    <t>Thirteen</t>
+  </si>
+  <si>
+    <t>Fourteen</t>
+  </si>
+  <si>
+    <t>Fifteen</t>
   </si>
 </sst>
 </file>
@@ -422,7 +467,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -477,111 +522,111 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8">
-        <v>1</v>
+      <c r="A8" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>13</v>
       </c>
       <c r="G9" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10">
-        <v>3</v>
+      <c r="A10" t="s">
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11">
-        <v>4</v>
+      <c r="A11" t="s">
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12">
-        <v>5</v>
+      <c r="A12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>8</v>
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14">
-        <v>7</v>
+      <c r="A14" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15">
-        <v>8</v>
+      <c r="A15" t="s">
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16">
-        <v>9</v>
+      <c r="A16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="F17">
-        <v>9</v>
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" t="s">
+        <v>21</v>
       </c>
       <c r="G17">
         <v>504</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18">
-        <v>11</v>
+      <c r="A18" t="s">
+        <v>23</v>
       </c>
       <c r="G18">
         <v>504</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19">
-        <v>12</v>
+      <c r="A19" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20">
-        <v>13</v>
-      </c>
-      <c r="E20">
-        <v>11</v>
+      <c r="A20" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21">
-        <v>14</v>
+      <c r="A21" t="s">
+        <v>26</v>
       </c>
       <c r="G21" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22">
-        <v>15</v>
+      <c r="A22" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>